<commit_message>
edited some pins with the same name (ie. gnd)
</commit_message>
<xml_diff>
--- a/Excel Sheet/PCI-Express x16.xlsx
+++ b/Excel Sheet/PCI-Express x16.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="20895" windowHeight="10170" activeTab="3"/>
@@ -15,12 +15,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One Column'!$B$2:$C$2</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="246">
   <si>
     <t xml:space="preserve">#  </t>
   </si>
@@ -500,6 +500,264 @@
   </si>
   <si>
     <t>Line</t>
+  </si>
+  <si>
+    <t>+12v _1</t>
+  </si>
+  <si>
+    <t>+12v _2</t>
+  </si>
+  <si>
+    <t>+12v _84</t>
+  </si>
+  <si>
+    <t>+12v _85</t>
+  </si>
+  <si>
+    <t>+3.3v _8</t>
+  </si>
+  <si>
+    <t>+3.3v _91</t>
+  </si>
+  <si>
+    <t>+3.3v _92</t>
+  </si>
+  <si>
+    <t>GND _4</t>
+  </si>
+  <si>
+    <t>GND _7</t>
+  </si>
+  <si>
+    <t>GND _13</t>
+  </si>
+  <si>
+    <t>GND _16</t>
+  </si>
+  <si>
+    <t>GND _18</t>
+  </si>
+  <si>
+    <t>GND _21</t>
+  </si>
+  <si>
+    <t>GND _22</t>
+  </si>
+  <si>
+    <t>GND _25</t>
+  </si>
+  <si>
+    <t>GND _26</t>
+  </si>
+  <si>
+    <t>GND _29</t>
+  </si>
+  <si>
+    <t>GND _32</t>
+  </si>
+  <si>
+    <t>GND _35</t>
+  </si>
+  <si>
+    <t>GND _36</t>
+  </si>
+  <si>
+    <t>GND _39</t>
+  </si>
+  <si>
+    <t>GND _40</t>
+  </si>
+  <si>
+    <t>GND _43</t>
+  </si>
+  <si>
+    <t>GND _44</t>
+  </si>
+  <si>
+    <t>GND _47</t>
+  </si>
+  <si>
+    <t>GND _49</t>
+  </si>
+  <si>
+    <t>GND _52</t>
+  </si>
+  <si>
+    <t>GND _53</t>
+  </si>
+  <si>
+    <t>GND _56</t>
+  </si>
+  <si>
+    <t>GND _57</t>
+  </si>
+  <si>
+    <t>GND _60</t>
+  </si>
+  <si>
+    <t>GND _61</t>
+  </si>
+  <si>
+    <t>GND _64</t>
+  </si>
+  <si>
+    <t>GND _65</t>
+  </si>
+  <si>
+    <t>GND _68</t>
+  </si>
+  <si>
+    <t>GND _69</t>
+  </si>
+  <si>
+    <t>GND _72</t>
+  </si>
+  <si>
+    <t>GND _73</t>
+  </si>
+  <si>
+    <t>GND _76</t>
+  </si>
+  <si>
+    <t>GND _77</t>
+  </si>
+  <si>
+    <t>GND _80</t>
+  </si>
+  <si>
+    <t>GND _86</t>
+  </si>
+  <si>
+    <t>GND _100</t>
+  </si>
+  <si>
+    <t>GND _105</t>
+  </si>
+  <si>
+    <t>GND _109</t>
+  </si>
+  <si>
+    <t>GND _113</t>
+  </si>
+  <si>
+    <t>GND _119</t>
+  </si>
+  <si>
+    <t>GND _123</t>
+  </si>
+  <si>
+    <t>GND _127</t>
+  </si>
+  <si>
+    <t>GND _131</t>
+  </si>
+  <si>
+    <t>GND _136</t>
+  </si>
+  <si>
+    <t>GND _140</t>
+  </si>
+  <si>
+    <t>GND _144</t>
+  </si>
+  <si>
+    <t>GND _148</t>
+  </si>
+  <si>
+    <t>GND _152</t>
+  </si>
+  <si>
+    <t>GND _156</t>
+  </si>
+  <si>
+    <t>GND _160</t>
+  </si>
+  <si>
+    <t>GND _164</t>
+  </si>
+  <si>
+    <t>GND  _94</t>
+  </si>
+  <si>
+    <t>GND  _97</t>
+  </si>
+  <si>
+    <t>GND  _102</t>
+  </si>
+  <si>
+    <t>GND  _106</t>
+  </si>
+  <si>
+    <t>GND  _110</t>
+  </si>
+  <si>
+    <t>GND  _116</t>
+  </si>
+  <si>
+    <t>GND  _120</t>
+  </si>
+  <si>
+    <t>GND  _124</t>
+  </si>
+  <si>
+    <t>GND  _128</t>
+  </si>
+  <si>
+    <t>GND  _133</t>
+  </si>
+  <si>
+    <t>GND  _137</t>
+  </si>
+  <si>
+    <t>GND  _141</t>
+  </si>
+  <si>
+    <t>GND  _145</t>
+  </si>
+  <si>
+    <t>GND  _149</t>
+  </si>
+  <si>
+    <t>GND  _153</t>
+  </si>
+  <si>
+    <t>GND  _157</t>
+  </si>
+  <si>
+    <t>GND  _161</t>
+  </si>
+  <si>
+    <t>RSVD _3</t>
+  </si>
+  <si>
+    <t>RSVD _30</t>
+  </si>
+  <si>
+    <t>RSVD _101</t>
+  </si>
+  <si>
+    <t>RSVD _114</t>
+  </si>
+  <si>
+    <t>RSVD _115</t>
+  </si>
+  <si>
+    <t>RSVD _132</t>
+  </si>
+  <si>
+    <t>RSVD  _12</t>
+  </si>
+  <si>
+    <t>PRSNT#2 _17</t>
+  </si>
+  <si>
+    <t>PRSNT#2 _31</t>
+  </si>
+  <si>
+    <t>PRSNT#2 _48</t>
+  </si>
+  <si>
+    <t>PRSNT#2 _81</t>
   </si>
 </sst>
 </file>
@@ -570,12 +828,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,22 +1143,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1125,14 +1383,14 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:7">
       <c r="B16">
@@ -2474,10 +2732,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:3" ht="15.75">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3814,42 +4072,42 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:12" ht="18.75">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4982,23 +5240,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="P33" workbookViewId="0">
+      <selection activeCell="AG67" sqref="AC4:AG67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:36" ht="18.75">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="1" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5105,7 +5363,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s">
         <v>158</v>
@@ -5120,7 +5378,7 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
       <c r="M4" t="s">
         <v>158</v>
@@ -5167,7 +5425,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="D5" t="s">
         <v>158</v>
@@ -5182,7 +5440,7 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="M5" t="s">
         <v>158</v>
@@ -5229,7 +5487,7 @@
         <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
         <v>158</v>
@@ -5244,7 +5502,7 @@
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="M6" t="s">
         <v>158</v>
@@ -5291,7 +5549,7 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="D7" t="s">
         <v>158</v>
@@ -5306,7 +5564,7 @@
         <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="M7" t="s">
         <v>158</v>
@@ -5353,7 +5611,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
         <v>158</v>
@@ -5368,7 +5626,7 @@
         <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="M8" t="s">
         <v>158</v>
@@ -5415,7 +5673,7 @@
         <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
         <v>158</v>
@@ -5430,7 +5688,7 @@
         <v>21</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
       <c r="M9" t="s">
         <v>158</v>
@@ -5477,7 +5735,7 @@
         <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
         <v>158</v>
@@ -5492,7 +5750,7 @@
         <v>22</v>
       </c>
       <c r="L10" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="M10" t="s">
         <v>158</v>
@@ -5507,7 +5765,7 @@
         <v>17</v>
       </c>
       <c r="U10" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="V10" t="s">
         <v>158</v>
@@ -5554,7 +5812,7 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="M11" t="s">
         <v>158</v>
@@ -5569,7 +5827,7 @@
         <v>31</v>
       </c>
       <c r="U11" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="V11" t="s">
         <v>158</v>
@@ -5601,7 +5859,7 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="M12" t="s">
         <v>158</v>
@@ -5616,7 +5874,7 @@
         <v>48</v>
       </c>
       <c r="U12" t="s">
-        <v>45</v>
+        <v>244</v>
       </c>
       <c r="V12" t="s">
         <v>158</v>
@@ -5648,7 +5906,7 @@
         <v>29</v>
       </c>
       <c r="L13" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="M13" t="s">
         <v>158</v>
@@ -5663,7 +5921,7 @@
         <v>81</v>
       </c>
       <c r="U13" t="s">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="V13" t="s">
         <v>158</v>
@@ -5695,7 +5953,7 @@
         <v>32</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="M14" t="s">
         <v>158</v>
@@ -5742,7 +6000,7 @@
         <v>35</v>
       </c>
       <c r="L15" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="M15" t="s">
         <v>158</v>
@@ -5789,7 +6047,7 @@
         <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="M16" t="s">
         <v>158</v>
@@ -5836,7 +6094,7 @@
         <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="M17" t="s">
         <v>158</v>
@@ -5851,7 +6109,7 @@
         <v>3</v>
       </c>
       <c r="U17" t="s">
-        <v>9</v>
+        <v>235</v>
       </c>
       <c r="V17" t="s">
         <v>158</v>
@@ -5883,7 +6141,7 @@
         <v>40</v>
       </c>
       <c r="L18" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
       <c r="M18" t="s">
         <v>158</v>
@@ -5898,7 +6156,7 @@
         <v>30</v>
       </c>
       <c r="U18" t="s">
-        <v>9</v>
+        <v>236</v>
       </c>
       <c r="V18" t="s">
         <v>158</v>
@@ -5930,7 +6188,7 @@
         <v>43</v>
       </c>
       <c r="L19" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="M19" t="s">
         <v>158</v>
@@ -5945,7 +6203,7 @@
         <v>101</v>
       </c>
       <c r="U19" t="s">
-        <v>9</v>
+        <v>237</v>
       </c>
       <c r="V19" t="s">
         <v>158</v>
@@ -5977,7 +6235,7 @@
         <v>44</v>
       </c>
       <c r="L20" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M20" t="s">
         <v>158</v>
@@ -5992,7 +6250,7 @@
         <v>114</v>
       </c>
       <c r="U20" t="s">
-        <v>9</v>
+        <v>238</v>
       </c>
       <c r="V20" t="s">
         <v>158</v>
@@ -6024,7 +6282,7 @@
         <v>47</v>
       </c>
       <c r="L21" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="M21" t="s">
         <v>158</v>
@@ -6039,7 +6297,7 @@
         <v>115</v>
       </c>
       <c r="U21" t="s">
-        <v>9</v>
+        <v>239</v>
       </c>
       <c r="V21" t="s">
         <v>158</v>
@@ -6071,7 +6329,7 @@
         <v>49</v>
       </c>
       <c r="L22" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="M22" t="s">
         <v>158</v>
@@ -6086,7 +6344,7 @@
         <v>132</v>
       </c>
       <c r="U22" t="s">
-        <v>9</v>
+        <v>240</v>
       </c>
       <c r="V22" t="s">
         <v>158</v>
@@ -6118,7 +6376,7 @@
         <v>52</v>
       </c>
       <c r="L23" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
       <c r="M23" t="s">
         <v>158</v>
@@ -6133,7 +6391,7 @@
         <v>12</v>
       </c>
       <c r="U23" t="s">
-        <v>37</v>
+        <v>241</v>
       </c>
       <c r="V23" t="s">
         <v>158</v>
@@ -6165,7 +6423,7 @@
         <v>53</v>
       </c>
       <c r="L24" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
       <c r="M24" t="s">
         <v>158</v>
@@ -6212,7 +6470,7 @@
         <v>56</v>
       </c>
       <c r="L25" t="s">
-        <v>11</v>
+        <v>188</v>
       </c>
       <c r="M25" t="s">
         <v>158</v>
@@ -6259,7 +6517,7 @@
         <v>57</v>
       </c>
       <c r="L26" t="s">
-        <v>11</v>
+        <v>189</v>
       </c>
       <c r="M26" t="s">
         <v>158</v>
@@ -6306,7 +6564,7 @@
         <v>60</v>
       </c>
       <c r="L27" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="M27" t="s">
         <v>158</v>
@@ -6353,7 +6611,7 @@
         <v>61</v>
       </c>
       <c r="L28" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="M28" t="s">
         <v>158</v>
@@ -6385,7 +6643,7 @@
         <v>64</v>
       </c>
       <c r="L29" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="M29" t="s">
         <v>158</v>
@@ -6417,7 +6675,7 @@
         <v>65</v>
       </c>
       <c r="L30" t="s">
-        <v>11</v>
+        <v>193</v>
       </c>
       <c r="M30" t="s">
         <v>158</v>
@@ -6449,7 +6707,7 @@
         <v>68</v>
       </c>
       <c r="L31" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="M31" t="s">
         <v>158</v>
@@ -6481,7 +6739,7 @@
         <v>69</v>
       </c>
       <c r="L32" t="s">
-        <v>11</v>
+        <v>195</v>
       </c>
       <c r="M32" t="s">
         <v>158</v>
@@ -6513,7 +6771,7 @@
         <v>72</v>
       </c>
       <c r="L33" t="s">
-        <v>11</v>
+        <v>196</v>
       </c>
       <c r="M33" t="s">
         <v>158</v>
@@ -6545,7 +6803,7 @@
         <v>73</v>
       </c>
       <c r="L34" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
       <c r="M34" t="s">
         <v>158</v>
@@ -6577,7 +6835,7 @@
         <v>76</v>
       </c>
       <c r="L35" t="s">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="M35" t="s">
         <v>158</v>
@@ -6609,7 +6867,7 @@
         <v>77</v>
       </c>
       <c r="L36" t="s">
-        <v>11</v>
+        <v>199</v>
       </c>
       <c r="M36" t="s">
         <v>158</v>
@@ -6641,7 +6899,7 @@
         <v>80</v>
       </c>
       <c r="L37" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="M37" t="s">
         <v>158</v>
@@ -6673,7 +6931,7 @@
         <v>86</v>
       </c>
       <c r="L38" t="s">
-        <v>11</v>
+        <v>201</v>
       </c>
       <c r="M38" t="s">
         <v>158</v>
@@ -6705,7 +6963,7 @@
         <v>100</v>
       </c>
       <c r="L39" t="s">
-        <v>11</v>
+        <v>202</v>
       </c>
       <c r="M39" t="s">
         <v>158</v>
@@ -6737,7 +6995,7 @@
         <v>105</v>
       </c>
       <c r="L40" t="s">
-        <v>11</v>
+        <v>203</v>
       </c>
       <c r="M40" t="s">
         <v>158</v>
@@ -6769,7 +7027,7 @@
         <v>109</v>
       </c>
       <c r="L41" t="s">
-        <v>11</v>
+        <v>204</v>
       </c>
       <c r="M41" t="s">
         <v>158</v>
@@ -6801,7 +7059,7 @@
         <v>113</v>
       </c>
       <c r="L42" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="M42" t="s">
         <v>158</v>
@@ -6833,7 +7091,7 @@
         <v>119</v>
       </c>
       <c r="L43" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="M43" t="s">
         <v>158</v>
@@ -6865,7 +7123,7 @@
         <v>123</v>
       </c>
       <c r="L44" t="s">
-        <v>11</v>
+        <v>207</v>
       </c>
       <c r="M44" t="s">
         <v>158</v>
@@ -6897,7 +7155,7 @@
         <v>127</v>
       </c>
       <c r="L45" t="s">
-        <v>11</v>
+        <v>208</v>
       </c>
       <c r="M45" t="s">
         <v>158</v>
@@ -6929,7 +7187,7 @@
         <v>131</v>
       </c>
       <c r="L46" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="M46" t="s">
         <v>158</v>
@@ -6961,7 +7219,7 @@
         <v>136</v>
       </c>
       <c r="L47" t="s">
-        <v>11</v>
+        <v>210</v>
       </c>
       <c r="M47" t="s">
         <v>158</v>
@@ -6993,7 +7251,7 @@
         <v>140</v>
       </c>
       <c r="L48" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="M48" t="s">
         <v>158</v>
@@ -7025,7 +7283,7 @@
         <v>144</v>
       </c>
       <c r="L49" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="M49" t="s">
         <v>158</v>
@@ -7057,7 +7315,7 @@
         <v>148</v>
       </c>
       <c r="L50" t="s">
-        <v>11</v>
+        <v>213</v>
       </c>
       <c r="M50" t="s">
         <v>158</v>
@@ -7089,7 +7347,7 @@
         <v>152</v>
       </c>
       <c r="L51" t="s">
-        <v>11</v>
+        <v>214</v>
       </c>
       <c r="M51" t="s">
         <v>158</v>
@@ -7121,7 +7379,7 @@
         <v>156</v>
       </c>
       <c r="L52" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
       <c r="M52" t="s">
         <v>158</v>
@@ -7153,7 +7411,7 @@
         <v>160</v>
       </c>
       <c r="L53" t="s">
-        <v>11</v>
+        <v>216</v>
       </c>
       <c r="M53" t="s">
         <v>158</v>
@@ -7185,7 +7443,7 @@
         <v>164</v>
       </c>
       <c r="L54" t="s">
-        <v>11</v>
+        <v>217</v>
       </c>
       <c r="M54" t="s">
         <v>158</v>
@@ -7217,7 +7475,7 @@
         <v>94</v>
       </c>
       <c r="L55" t="s">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="M55" t="s">
         <v>158</v>
@@ -7249,7 +7507,7 @@
         <v>97</v>
       </c>
       <c r="L56" t="s">
-        <v>39</v>
+        <v>219</v>
       </c>
       <c r="M56" t="s">
         <v>158</v>
@@ -7281,7 +7539,7 @@
         <v>102</v>
       </c>
       <c r="L57" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="M57" t="s">
         <v>158</v>
@@ -7313,7 +7571,7 @@
         <v>106</v>
       </c>
       <c r="L58" t="s">
-        <v>39</v>
+        <v>221</v>
       </c>
       <c r="M58" t="s">
         <v>158</v>
@@ -7345,7 +7603,7 @@
         <v>110</v>
       </c>
       <c r="L59" t="s">
-        <v>39</v>
+        <v>222</v>
       </c>
       <c r="M59" t="s">
         <v>158</v>
@@ -7377,7 +7635,7 @@
         <v>116</v>
       </c>
       <c r="L60" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="M60" t="s">
         <v>158</v>
@@ -7409,7 +7667,7 @@
         <v>120</v>
       </c>
       <c r="L61" t="s">
-        <v>39</v>
+        <v>224</v>
       </c>
       <c r="M61" t="s">
         <v>158</v>
@@ -7441,7 +7699,7 @@
         <v>124</v>
       </c>
       <c r="L62" t="s">
-        <v>39</v>
+        <v>225</v>
       </c>
       <c r="M62" t="s">
         <v>158</v>
@@ -7473,7 +7731,7 @@
         <v>128</v>
       </c>
       <c r="L63" t="s">
-        <v>39</v>
+        <v>226</v>
       </c>
       <c r="M63" t="s">
         <v>158</v>
@@ -7505,7 +7763,7 @@
         <v>133</v>
       </c>
       <c r="L64" t="s">
-        <v>39</v>
+        <v>227</v>
       </c>
       <c r="M64" t="s">
         <v>158</v>
@@ -7537,7 +7795,7 @@
         <v>137</v>
       </c>
       <c r="L65" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="M65" t="s">
         <v>158</v>
@@ -7569,7 +7827,7 @@
         <v>141</v>
       </c>
       <c r="L66" t="s">
-        <v>39</v>
+        <v>229</v>
       </c>
       <c r="M66" t="s">
         <v>158</v>
@@ -7601,7 +7859,7 @@
         <v>145</v>
       </c>
       <c r="L67" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="M67" t="s">
         <v>158</v>
@@ -7633,7 +7891,7 @@
         <v>149</v>
       </c>
       <c r="L68" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
       <c r="M68" t="s">
         <v>158</v>
@@ -7650,7 +7908,7 @@
         <v>153</v>
       </c>
       <c r="L69" t="s">
-        <v>39</v>
+        <v>232</v>
       </c>
       <c r="M69" t="s">
         <v>158</v>
@@ -7667,7 +7925,7 @@
         <v>157</v>
       </c>
       <c r="L70" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="M70" t="s">
         <v>158</v>
@@ -7684,7 +7942,7 @@
         <v>161</v>
       </c>
       <c r="L71" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
       <c r="M71" t="s">
         <v>158</v>

</xml_diff>